<commit_message>
Update master data with new DAF values
</commit_message>
<xml_diff>
--- a/data/inputs/Artikel & Materialien FGR+.XLSX
+++ b/data/inputs/Artikel & Materialien FGR+.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uklra\Downloads\ddmrp_mvp_monorepo\backend\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B79BA7B-12E2-475B-BC3F-324A4771EEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F3E3D8-9195-4098-97F3-91A82809DEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -545,8 +545,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -959,7 +959,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="2">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -1011,7 +1011,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="2">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="D18" s="2">
         <v>3</v>
@@ -1089,7 +1089,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="2">
-        <v>1</v>
+        <v>1.9</v>
       </c>
       <c r="D21" s="2">
         <v>4</v>
@@ -1141,7 +1141,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="2">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D23" s="2">
         <v>3</v>
@@ -1167,7 +1167,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="2">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="D24" s="2">
         <v>3</v>
@@ -1193,7 +1193,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="2">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="D25" s="2">
         <v>3</v>
@@ -1245,7 +1245,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="2">
-        <v>1</v>
+        <v>1.7</v>
       </c>
       <c r="D27" s="2">
         <v>3</v>
@@ -1271,7 +1271,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="2">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="D28" s="2">
         <v>3</v>
@@ -1297,7 +1297,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="2">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="D29" s="2">
         <v>3</v>
@@ -1323,7 +1323,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="2">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="D30" s="2">
         <v>3</v>
@@ -1349,7 +1349,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="2">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="D31" s="2">
         <v>3</v>
@@ -1401,7 +1401,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="2">
-        <v>1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D33" s="2">
         <v>3</v>
@@ -1476,8 +1476,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>